<commit_message>
Changes to Excel Reader
</commit_message>
<xml_diff>
--- a/UploadedFiles/MockData.xlsx
+++ b/UploadedFiles/MockData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vchidrawar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEBC4BAA-1A21-41A1-98F0-D2D69D4AE316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F5386D-366A-45CA-9AB5-16757E08A92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8F3B570-1DEE-450D-9DF2-53FB1A6FAA17}"/>
+    <workbookView xWindow="-23148" yWindow="4560" windowWidth="23256" windowHeight="12576" xr2:uid="{B8F3B570-1DEE-450D-9DF2-53FB1A6FAA17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,37 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
-  <si>
-    <t>Addy 1</t>
-  </si>
-  <si>
-    <t>Addy 2</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State/Province</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
-    <t>BuildingName</t>
-  </si>
-  <si>
-    <t>FloorNumber</t>
-  </si>
-  <si>
-    <t>OfficeType</t>
-  </si>
-  <si>
-    <t>OfficeCode</t>
-  </si>
-  <si>
-    <t>SquareFeet</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
   <si>
     <t>KPS Tech Campus</t>
   </si>
@@ -77,9 +47,6 @@
   </si>
   <si>
     <t>New Jersey</t>
-  </si>
-  <si>
-    <t>AreaName</t>
   </si>
   <si>
     <t>Holtec USA - Camden</t>
@@ -131,12 +98,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,8 +148,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,310 +472,316 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>12345</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" s="4">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5">
+        <v>501</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" s="1">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5">
+        <v>502</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>12345</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="I3" s="5">
+        <v>601</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12345</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5">
+        <v>602</v>
+      </c>
+      <c r="J4" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>12345</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>501</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>12345</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>502</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>12345</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>601</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
       </c>
       <c r="K4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>12345</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>101</v>
+      </c>
+      <c r="J5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5">
+      <c r="K5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
         <v>12345</v>
       </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>602</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <v>102</v>
+      </c>
+      <c r="J6" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>12345</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>101</v>
-      </c>
-      <c r="J6" t="s">
-        <v>23</v>
       </c>
       <c r="K6">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1">
+        <v>67890</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>101</v>
+      </c>
+      <c r="J7" t="s">
         <v>13</v>
       </c>
-      <c r="F7">
-        <v>12345</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>102</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
       <c r="K7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1">
         <v>67890</v>
       </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>101</v>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>104</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1">
         <v>67890</v>
       </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
+      <c r="G9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
         <v>104</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K9">
         <v>5</v>
@@ -782,5 +790,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
8/16/2022 - Excel Reader modified
</commit_message>
<xml_diff>
--- a/UploadedFiles/MockData.xlsx
+++ b/UploadedFiles/MockData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vchidrawar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F5386D-366A-45CA-9AB5-16757E08A92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FE499D-B2AB-4A51-8E38-E5ED747B5FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="4560" windowWidth="23256" windowHeight="12576" xr2:uid="{B8F3B570-1DEE-450D-9DF2-53FB1A6FAA17}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t>KPS Tech Campus</t>
   </si>
@@ -469,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E1B0C5-1787-4BB0-872A-4A970CBC6C49}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,39 +754,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1">
-        <v>67890</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
-        <v>104</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>